<commit_message>
Centenary Trophy - Medal
</commit_message>
<xml_diff>
--- a/data/leaguedata.xlsx
+++ b/data/leaguedata.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="33">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -90,6 +90,18 @@
     <t xml:space="preserve">40</t>
   </si>
   <si>
+    <t xml:space="preserve">Centenary Trophy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19/4/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centenary Trophy - Medal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/R</t>
+  </si>
+  <si>
     <t xml:space="preserve">Key</t>
   </si>
   <si>
@@ -99,7 +111,34 @@
     <t xml:space="preserve">Next Competition</t>
   </si>
   <si>
-    <t xml:space="preserve">Saturday 19th April - Centenary Trophy - Medal</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Pros Roll Up Week 2 - 24</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> April</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Table 1</t>
@@ -120,7 +159,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -144,6 +183,18 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="0"/>
@@ -267,7 +318,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -292,6 +343,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -328,7 +383,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -372,7 +427,6 @@
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
@@ -388,7 +442,6 @@
           <bgColor rgb="FF808080"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
 </styleSheet>
@@ -574,7 +627,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -871,7 +924,9 @@
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="5" t="n">
+        <v>41</v>
+      </c>
       <c r="C10" s="5" t="n">
         <v>18</v>
       </c>
@@ -901,7 +956,9 @@
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5" t="n">
+        <v>39</v>
+      </c>
       <c r="C11" s="5" t="n">
         <v>18</v>
       </c>
@@ -931,7 +988,9 @@
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="C12" s="5" t="n">
         <v>15</v>
       </c>
@@ -958,40 +1017,94 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>71</v>
+      </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="5"/>
+      <c r="D13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="5" t="n">
+        <v>82</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>75</v>
+      </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="5"/>
+      <c r="D14" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="5" t="n">
+        <v>92</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="5"/>
+      <c r="D15" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
@@ -1282,40 +1395,40 @@
       <c r="J39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="8"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="11"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="12"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="14"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
@@ -1346,7 +1459,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1358,10 +1471,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -1376,10 +1489,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1462,93 +1575,93 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="A1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" customFormat="false" ht="15.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
     </row>
     <row r="3" customFormat="false" ht="15.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="19" t="n">
+      <c r="B3" s="20" t="n">
         <v>12.7</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" customFormat="false" ht="14.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" customFormat="false" ht="14.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" customFormat="false" ht="14.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" customFormat="false" ht="14.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" customFormat="false" ht="14.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
     </row>
     <row r="9" customFormat="false" ht="14.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
     </row>
     <row r="10" customFormat="false" ht="14.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Pros Roll Up Week 2
</commit_message>
<xml_diff>
--- a/data/leaguedata.xlsx
+++ b/data/leaguedata.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="37">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -81,15 +81,18 @@
     <t xml:space="preserve">12/4/2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Pros Roll Up Stableford WK 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17/4/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pros Roll Up Stableford</t>
   </si>
   <si>
-    <t xml:space="preserve">17/4/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40</t>
-  </si>
-  <si>
     <t xml:space="preserve">Centenary Trophy</t>
   </si>
   <si>
@@ -100,6 +103,15 @@
   </si>
   <si>
     <t xml:space="preserve">N/R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pros Roll Up Stableford – WK 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24/04/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pros Roll Up Stableford WK 2</t>
   </si>
   <si>
     <t xml:space="preserve">Key</t>
@@ -159,7 +171,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -187,11 +199,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
@@ -318,7 +325,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -343,10 +350,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -383,7 +386,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -627,7 +630,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1001,7 +1004,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G12" s="5" t="n">
         <v>1</v>
@@ -1030,17 +1033,17 @@
       <c r="E13" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>22</v>
+      <c r="F13" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="G13" s="5" t="n">
         <v>3</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="6" t="s">
         <v>24</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="J13" s="5" t="n">
         <v>82</v>
@@ -1060,17 +1063,17 @@
       <c r="E14" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>22</v>
+      <c r="F14" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="G14" s="5" t="n">
         <v>2</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" s="6" t="s">
         <v>24</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="J14" s="5" t="n">
         <v>92</v>
@@ -1090,45 +1093,85 @@
       <c r="E15" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>22</v>
+      <c r="F15" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="G15" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="I15" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="J15" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="5"/>
+      <c r="A16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="5" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="5"/>
+      <c r="A17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="5" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3"/>
@@ -1395,40 +1438,40 @@
       <c r="J39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="9"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="12"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="11"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="13"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="15"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
@@ -1471,10 +1514,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -1489,10 +1532,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1575,93 +1618,93 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="A1" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="15.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="B2" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" customFormat="false" ht="15.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="20" t="n">
+      <c r="B3" s="19" t="n">
         <v>12.7</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" customFormat="false" ht="14.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="14.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" customFormat="false" ht="14.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="14.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="14.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
     </row>
     <row r="9" customFormat="false" ht="14.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" customFormat="false" ht="14.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>